<commit_message>
feat: complete page 1 coordinates
</commit_message>
<xml_diff>
--- a/data/samples/sample_data_form_le1.xlsx
+++ b/data/samples/sample_data_form_le1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhammad.junaidi\Documents\Streamlit Apps\form_LE1_auto_fill\data\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A336C94-6567-483B-8D3E-F8000D3DB621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960531AB-1F3A-408A-81AC-0450F2D11F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="990" yWindow="930" windowWidth="18110" windowHeight="10190" xr2:uid="{E9781D6C-8669-4BFF-9D9D-C5AC75C60674}"/>
+    <workbookView xWindow="-4290" yWindow="-11535" windowWidth="18105" windowHeight="10185" xr2:uid="{E9781D6C-8669-4BFF-9D9D-C5AC75C60674}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -775,15 +775,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F4ACDE8-16CB-4AA9-9044-716AA541F9D0}">
   <dimension ref="A1:CF3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.81640625" customWidth="1"/>
-    <col min="3" max="3" width="25.54296875" customWidth="1"/>
+    <col min="3" max="3" width="45.26953125" customWidth="1"/>
     <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.54296875" customWidth="1"/>
     <col min="6" max="6" width="9.36328125" customWidth="1"/>

</xml_diff>

<commit_message>
feat: complete page 3 coordinates
</commit_message>
<xml_diff>
--- a/data/samples/sample_data_form_le1.xlsx
+++ b/data/samples/sample_data_form_le1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhammad.junaidi\Documents\Streamlit Apps\form_LE1_auto_fill\data\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960531AB-1F3A-408A-81AC-0450F2D11F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0DB96C-510F-4347-A3F4-FE6B4D5E7D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4290" yWindow="-11535" windowWidth="18105" windowHeight="10185" xr2:uid="{E9781D6C-8669-4BFF-9D9D-C5AC75C60674}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{E9781D6C-8669-4BFF-9D9D-C5AC75C60674}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -775,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F4ACDE8-16CB-4AA9-9044-716AA541F9D0}">
   <dimension ref="A1:CF3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AG7" sqref="AG7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -796,6 +796,7 @@
     <col min="36" max="36" width="11.6328125" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.81640625" customWidth="1"/>
     <col min="57" max="57" width="26.54296875" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="14.26953125" customWidth="1"/>
     <col min="60" max="60" width="25.7265625" bestFit="1" customWidth="1"/>

</xml_diff>